<commit_message>
icon 64x64 added, and manifest changed
</commit_message>
<xml_diff>
--- a/CarbonoWebAddin-master/CarbonoTemplatesAddIn/CarbonoTemplatesAddIn/bin/Debug/Book1.xlsx
+++ b/CarbonoWebAddin-master/CarbonoTemplatesAddIn/CarbonoTemplatesAddIn/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R81f7b4e9c6814243"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R93f32350efdf4a60"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R3b19b82925294425"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5f23f4bc67174b91"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7df16fd7-5513-4b12-8b2a-c20f477fd482}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d5057204-7204-487e-8627-8814d7d10bb7}">
   <we:reference id="72938ba6-ac96-4dfa-ad27-61e4e3f3ba77" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Pop up de informação adicionado
</commit_message>
<xml_diff>
--- a/CarbonoWebAddin-master/CarbonoTemplatesAddIn/CarbonoTemplatesAddIn/bin/Debug/Book1.xlsx
+++ b/CarbonoWebAddin-master/CarbonoTemplatesAddIn/CarbonoTemplatesAddIn/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R93f32350efdf4a60"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Folha1" sheetId="1" r:id="Rd856c2549c52458a"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5f23f4bc67174b91"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc4cdabe8b9894e70"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d5057204-7204-487e-8627-8814d7d10bb7}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1659a75b-73f7-45a9-a397-caf6b0895941}">
   <we:reference id="72938ba6-ac96-4dfa-ad27-61e4e3f3ba77" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Infopage case sensitive 1 fixed
</commit_message>
<xml_diff>
--- a/CarbonoWebAddin-master/CarbonoTemplatesAddIn/CarbonoTemplatesAddIn/bin/Debug/Book1.xlsx
+++ b/CarbonoWebAddin-master/CarbonoTemplatesAddIn/CarbonoTemplatesAddIn/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Folha1" sheetId="1" r:id="Rd856c2549c52458a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Folha1" sheetId="1" r:id="R8839e88d00774631"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc4cdabe8b9894e70"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R381dcc293d47458c"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1659a75b-73f7-45a9-a397-caf6b0895941}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ba9b782d-ce11-49fe-95cf-b4213e1cccc9}">
   <we:reference id="72938ba6-ac96-4dfa-ad27-61e4e3f3ba77" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>